<commit_message>
Se añade mensaje de cantidad de registros realizados por medio de excel
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarInscripcionEstudiantes.xlsx
+++ b/storage/app/plantillaExcel/ImportarInscripcionEstudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\Desktop\Proyectos UES\SIGEN\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BC495E-2597-43B3-8F34-89ACA91A5447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C76080-0806-4C49-AE3B-316108D5790C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="360" windowWidth="24240" windowHeight="13260" xr2:uid="{AE4FFBD4-C56E-47BF-9535-B66E31E7AF2B}"/>
+    <workbookView xWindow="2460" yWindow="645" windowWidth="18885" windowHeight="11235" xr2:uid="{AE4FFBD4-C56E-47BF-9535-B66E31E7AF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,25 @@
     <t>CODIGO</t>
   </si>
   <si>
-    <t>DESCRIPCION: INSCRIPCION DE ESTUDIANTES</t>
-  </si>
-  <si>
     <t>PI01</t>
   </si>
   <si>
     <t>Carnet de estudiantes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DESCRIPCION: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plantilla que se encarga de inscribir estudiantes en una materia para un ciclo/periodo, ingrese el carnet del estudiante en MAYUSCULAS</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -238,6 +250,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -261,9 +276,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,40 +591,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E0CBDF-F575-4A03-8A7D-75D5844D3D4C}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -620,7 +633,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -691,6 +704,390 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -698,5 +1095,6 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>